<commit_message>
All files for publication
All analysis scripts and files associated with publication in fisheries research - 2020
</commit_message>
<xml_diff>
--- a/Manuscript/Submitted Files to FR/R2 - 20 July 2020/Manuscript Pieces/Figures and Tables/Table 3 - Bayesian Parameter Estimates.xlsx
+++ b/Manuscript/Submitted Files to FR/R2 - 20 July 2020/Manuscript Pieces/Figures and Tables/Table 3 - Bayesian Parameter Estimates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Weng Lab/Personal_Folders/Steve/dissertation work/Ch 4. Opakapaka Growth/Manuscript/Submitted Files to FR/Revised Manuscript Files/Figures and Tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Weng Lab/Personal_Folders/Steve/dissertation work/Ch 4. Opakapaka Growth/Manuscript/Submitted Files to FR/R2 - 20 July 2020/Manuscript Pieces/Figures and Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F449E357-BAD2-0741-8EB7-CC70D04A24F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BBC9A1-4375-6C49-A420-974BBC1BCD18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="460" windowWidth="23200" windowHeight="16280"/>
+    <workbookView xWindow="6800" yWindow="460" windowWidth="23200" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 2 - Bayesian Parameter Es" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -96,7 +98,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -613,7 +615,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -646,6 +648,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="18" fillId="33" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="18" fillId="33" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
@@ -1009,11 +1023,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="M43" sqref="M43"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1061,32 +1075,32 @@
       <c r="N1" s="13"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="22" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="6">
-        <v>61.346223718055903</v>
+        <v>61.414267231220002</v>
       </c>
       <c r="D2" s="6">
-        <v>1.7663447021623999</v>
+        <v>1.82920203319375</v>
       </c>
       <c r="E2" s="6">
-        <v>58.161829628287002</v>
+        <v>58.087532293135702</v>
       </c>
       <c r="F2" s="6">
-        <v>61.2633865763191</v>
+        <v>61.309592452613302</v>
       </c>
       <c r="G2" s="6">
-        <v>65.028730297672197</v>
+        <v>65.235295591005695</v>
       </c>
       <c r="H2" s="6">
-        <v>1.0033084918125399</v>
-      </c>
-      <c r="I2" s="6">
-        <v>2000</v>
+        <v>1.00257691244239</v>
+      </c>
+      <c r="I2" s="18">
+        <v>1600</v>
       </c>
       <c r="J2" s="13"/>
       <c r="K2" s="13"/>
@@ -1095,30 +1109,30 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="19"/>
+      <c r="A3" s="23"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="6">
-        <v>5.2945437439361802</v>
+        <v>5.2948566901515601</v>
       </c>
       <c r="D3" s="6">
-        <v>0.35173140329411301</v>
+        <v>0.35190761770588003</v>
       </c>
       <c r="E3" s="6">
-        <v>4.6098723515659001</v>
+        <v>4.6131158297289403</v>
       </c>
       <c r="F3" s="6">
-        <v>5.2924929813413799</v>
+        <v>5.29275391157213</v>
       </c>
       <c r="G3" s="6">
-        <v>5.9927724511989302</v>
+        <v>5.9944060394688199</v>
       </c>
       <c r="H3" s="6">
-        <v>1.0010180692170401</v>
-      </c>
-      <c r="I3" s="6">
-        <v>36000</v>
+        <v>1.00106331693892</v>
+      </c>
+      <c r="I3" s="18">
+        <v>26000</v>
       </c>
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
@@ -1127,30 +1141,30 @@
       <c r="N3" s="13"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="19"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="6">
-        <v>3.6155220152994702E-2</v>
+        <v>3.6150765221975502E-2</v>
       </c>
       <c r="D4" s="6">
-        <v>4.9101976505464299E-3</v>
+        <v>4.9040009563587998E-3</v>
       </c>
       <c r="E4" s="6">
-        <v>2.7844820640491201E-2</v>
+        <v>2.7829646234870799E-2</v>
       </c>
       <c r="F4" s="6">
-        <v>3.5700920873678002E-2</v>
+        <v>3.5697400883875498E-2</v>
       </c>
       <c r="G4" s="6">
-        <v>4.7056779387938001E-2</v>
+        <v>4.6990631480184099E-2</v>
       </c>
       <c r="H4" s="6">
-        <v>1.0010180692170401</v>
-      </c>
-      <c r="I4" s="6">
-        <v>36000</v>
+        <v>1.00106331693892</v>
+      </c>
+      <c r="I4" s="18">
+        <v>26000</v>
       </c>
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
@@ -1159,29 +1173,29 @@
       <c r="N4" s="13"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="19"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="6">
-        <v>31.216115417476502</v>
+        <v>31.1381248409362</v>
       </c>
       <c r="D5" s="6">
-        <v>5.3367940290299201</v>
+        <v>5.3461058285052001</v>
       </c>
       <c r="E5" s="6">
-        <v>22.442419279887499</v>
+        <v>22.3912753756623</v>
       </c>
       <c r="F5" s="6">
-        <v>30.642272001200698</v>
+        <v>30.559168660160001</v>
       </c>
       <c r="G5" s="6">
-        <v>43.427149751591301</v>
+        <v>43.450750942527797</v>
       </c>
       <c r="H5" s="6">
-        <v>1.0021888512164701</v>
-      </c>
-      <c r="I5" s="6">
+        <v>1.0017729921254099</v>
+      </c>
+      <c r="I5" s="18">
         <v>2500</v>
       </c>
       <c r="J5" s="13"/>
@@ -1191,30 +1205,30 @@
       <c r="N5" s="13"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="19"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="6">
-        <v>3403.9479869981701</v>
+        <v>3404.4547780647699</v>
       </c>
       <c r="D6" s="6">
-        <v>104.182608429456</v>
+        <v>105.133030120396</v>
       </c>
       <c r="E6" s="6">
-        <v>3187.0474083396298</v>
+        <v>3185.3707474586799</v>
       </c>
       <c r="F6" s="6">
-        <v>3408.5751246720502</v>
+        <v>3408.41235216103</v>
       </c>
       <c r="G6" s="6">
-        <v>3594.16615222373</v>
+        <v>3597.4777060022002</v>
       </c>
       <c r="H6" s="6">
-        <v>1.0017565582960799</v>
-      </c>
-      <c r="I6" s="6">
-        <v>3700</v>
+        <v>1.0018106148192001</v>
+      </c>
+      <c r="I6" s="18">
+        <v>2400</v>
       </c>
       <c r="J6" s="13"/>
       <c r="K6" s="13"/>
@@ -1223,30 +1237,30 @@
       <c r="N6" s="13"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="19"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="6">
-        <v>0.295082370317374</v>
+        <v>0.294167736107174</v>
       </c>
       <c r="D7" s="6">
-        <v>2.7202203326414699E-2</v>
+        <v>2.8047742173438299E-2</v>
       </c>
       <c r="E7" s="6">
-        <v>0.24454933562020301</v>
+        <v>0.24217961638458699</v>
       </c>
       <c r="F7" s="6">
-        <v>0.293927438510104</v>
+        <v>0.293518322402951</v>
       </c>
       <c r="G7" s="6">
-        <v>0.35047965373067202</v>
+        <v>0.35192945236529399</v>
       </c>
       <c r="H7" s="6">
-        <v>1.0035974904218801</v>
-      </c>
-      <c r="I7" s="6">
-        <v>1800</v>
+        <v>1.00315038681786</v>
+      </c>
+      <c r="I7" s="18">
+        <v>1400</v>
       </c>
       <c r="J7" s="13"/>
       <c r="K7" s="13"/>
@@ -1255,30 +1269,30 @@
       <c r="N7" s="13"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="19"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="6">
-        <v>9.1153158553782896E-3</v>
+        <v>9.0691925528591892E-3</v>
       </c>
       <c r="D8" s="6">
-        <v>3.1886681477011E-3</v>
+        <v>3.1715882420971201E-3</v>
       </c>
       <c r="E8" s="6">
-        <v>4.6751016937372899E-3</v>
+        <v>4.6774165395736898E-3</v>
       </c>
       <c r="F8" s="6">
-        <v>8.5120432342749106E-3</v>
+        <v>8.4602060723531994E-3</v>
       </c>
       <c r="G8" s="6">
-        <v>1.6868067274900599E-2</v>
+        <v>1.6901688780413201E-2</v>
       </c>
       <c r="H8" s="6">
-        <v>1.00100751564337</v>
-      </c>
-      <c r="I8" s="6">
-        <v>38000</v>
+        <v>1.0013049935035401</v>
+      </c>
+      <c r="I8" s="18">
+        <v>6300</v>
       </c>
       <c r="J8" s="13"/>
       <c r="K8" s="13"/>
@@ -1287,30 +1301,30 @@
       <c r="N8" s="13"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="19"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="6">
-        <v>16638.556094895401</v>
+        <v>16745.571442881901</v>
       </c>
       <c r="D9" s="6">
-        <v>11206.635246631</v>
+        <v>11200.938522971899</v>
       </c>
       <c r="E9" s="6">
-        <v>3514.5469644550399</v>
+        <v>3500.5783210760201</v>
       </c>
       <c r="F9" s="6">
-        <v>13801.6928562173</v>
+        <v>13971.3417739938</v>
       </c>
       <c r="G9" s="6">
-        <v>45752.820890610099</v>
+        <v>45707.546103332403</v>
       </c>
       <c r="H9" s="6">
-        <v>1.00100751564337</v>
-      </c>
-      <c r="I9" s="6">
-        <v>38000</v>
+        <v>1.0013049935035401</v>
+      </c>
+      <c r="I9" s="18">
+        <v>6300</v>
       </c>
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
@@ -1319,30 +1333,30 @@
       <c r="N9" s="13"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="19"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="6">
-        <v>11.754392736136399</v>
+        <v>11.7016484759873</v>
       </c>
       <c r="D10" s="6">
-        <v>1.8401877163127101</v>
+        <v>1.8196589291897001</v>
       </c>
       <c r="E10" s="6">
-        <v>8.7239669835117706</v>
+        <v>8.6928893416442499</v>
       </c>
       <c r="F10" s="6">
-        <v>11.5531673408501</v>
+        <v>11.511457237706599</v>
       </c>
       <c r="G10" s="6">
-        <v>15.937397945174499</v>
+        <v>15.8362197734214</v>
       </c>
       <c r="H10" s="6">
-        <v>1.0016430474776501</v>
-      </c>
-      <c r="I10" s="6">
-        <v>2800</v>
+        <v>1.0014624521326501</v>
+      </c>
+      <c r="I10" s="18">
+        <v>4200</v>
       </c>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
@@ -1351,30 +1365,30 @@
       <c r="N10" s="13"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="19"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="6">
-        <v>0.21231079530053801</v>
+        <v>0.21230013838112799</v>
       </c>
       <c r="D11" s="6">
-        <v>3.1119761141019199E-2</v>
+        <v>3.1328805504893503E-2</v>
       </c>
       <c r="E11" s="6">
-        <v>0.16097765490000901</v>
+        <v>0.16048437793214099</v>
       </c>
       <c r="F11" s="6">
-        <v>0.20898875478411499</v>
+        <v>0.20906687996984399</v>
       </c>
       <c r="G11" s="6">
-        <v>0.28191104357755897</v>
+        <v>0.28274407224165099</v>
       </c>
       <c r="H11" s="6">
-        <v>1.0016434366839599</v>
-      </c>
-      <c r="I11" s="6">
-        <v>5700</v>
+        <v>1.0015830115165001</v>
+      </c>
+      <c r="I11" s="18">
+        <v>3300</v>
       </c>
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
@@ -1383,30 +1397,30 @@
       <c r="N11" s="13"/>
     </row>
     <row r="12" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="7">
-        <v>4.8082455969554401</v>
+        <v>4.8098301321354402</v>
       </c>
       <c r="D12" s="7">
-        <v>0.68371581336070497</v>
+        <v>0.68894357480175705</v>
       </c>
       <c r="E12" s="7">
-        <v>3.5472182547714901</v>
+        <v>3.5367673389995402</v>
       </c>
       <c r="F12" s="7">
-        <v>4.7849464485924003</v>
+        <v>4.7831583852221797</v>
       </c>
       <c r="G12" s="7">
-        <v>6.2120422901001202</v>
+        <v>6.2311360948966499</v>
       </c>
       <c r="H12" s="7">
-        <v>1.0016434366839599</v>
-      </c>
-      <c r="I12" s="7">
-        <v>5700</v>
+        <v>1.0015830115165001</v>
+      </c>
+      <c r="I12" s="19">
+        <v>3300</v>
       </c>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
@@ -1415,32 +1429,32 @@
       <c r="N12" s="13"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="22" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="6">
-        <v>61.6297582143238</v>
+        <v>61.7914316414209</v>
       </c>
       <c r="D13" s="6">
-        <v>1.84010467028606</v>
+        <v>1.7966963667795399</v>
       </c>
       <c r="E13" s="6">
-        <v>58.346997299154502</v>
+        <v>58.520674101800097</v>
       </c>
       <c r="F13" s="6">
-        <v>61.521416334807398</v>
+        <v>61.692245326494401</v>
       </c>
       <c r="G13" s="6">
-        <v>65.601140059394993</v>
+        <v>65.616737723187597</v>
       </c>
       <c r="H13" s="6">
-        <v>1.0015284224317</v>
-      </c>
-      <c r="I13" s="6">
-        <v>30000</v>
+        <v>1.0025007497173499</v>
+      </c>
+      <c r="I13" s="18">
+        <v>1300</v>
       </c>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
@@ -1449,30 +1463,30 @@
       <c r="N13" s="13"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="19"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="6">
-        <v>5.3295995457470102</v>
+        <v>5.3266710454401203</v>
       </c>
       <c r="D14" s="6">
-        <v>0.34795556536142702</v>
+        <v>0.34876270373845297</v>
       </c>
       <c r="E14" s="6">
-        <v>4.6583054486396396</v>
+        <v>4.64972619132205</v>
       </c>
       <c r="F14" s="6">
-        <v>5.3247168276874302</v>
+        <v>5.3232537325172196</v>
       </c>
       <c r="G14" s="6">
-        <v>6.0250136082762697</v>
+        <v>6.0216735482716599</v>
       </c>
       <c r="H14" s="6">
-        <v>1.0009925972359199</v>
-      </c>
-      <c r="I14" s="6">
-        <v>84000</v>
+        <v>1.0010161136939799</v>
+      </c>
+      <c r="I14" s="18">
+        <v>64000</v>
       </c>
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
@@ -1481,30 +1495,30 @@
       <c r="N14" s="13"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="19"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="6">
-        <v>3.5662447384742099E-2</v>
+        <v>3.5704986138749603E-2</v>
       </c>
       <c r="D15" s="6">
-        <v>4.7298770371475597E-3</v>
+        <v>4.7580220737640797E-3</v>
       </c>
       <c r="E15" s="6">
-        <v>2.7547610619518902E-2</v>
+        <v>2.7578178929021199E-2</v>
       </c>
       <c r="F15" s="6">
-        <v>3.5270122393084802E-2</v>
+        <v>3.5289513028937E-2</v>
       </c>
       <c r="G15" s="6">
-        <v>4.6083353540835398E-2</v>
+        <v>4.6253568161681503E-2</v>
       </c>
       <c r="H15" s="6">
-        <v>1.0009925972359199</v>
-      </c>
-      <c r="I15" s="6">
-        <v>84000</v>
+        <v>1.0010161136939799</v>
+      </c>
+      <c r="I15" s="18">
+        <v>64000</v>
       </c>
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
@@ -1513,30 +1527,30 @@
       <c r="N15" s="13"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="19"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="6">
-        <v>30.8549657356238</v>
+        <v>31.114592884433002</v>
       </c>
       <c r="D16" s="6">
-        <v>5.0185449590861202</v>
+        <v>5.08621286736311</v>
       </c>
       <c r="E16" s="6">
-        <v>22.5044622288118</v>
+        <v>22.683899505371102</v>
       </c>
       <c r="F16" s="6">
-        <v>30.330483238558099</v>
+        <v>30.591386804450501</v>
       </c>
       <c r="G16" s="6">
-        <v>42.169971485995099</v>
+        <v>42.692884600331901</v>
       </c>
       <c r="H16" s="6">
-        <v>1.0019151399517201</v>
-      </c>
-      <c r="I16" s="6">
-        <v>7900</v>
+        <v>1.00162190637336</v>
+      </c>
+      <c r="I16" s="18">
+        <v>3100</v>
       </c>
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
@@ -1545,30 +1559,30 @@
       <c r="N16" s="13"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="19"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="6">
-        <v>3407.2614012081899</v>
+        <v>3413.1938514162198</v>
       </c>
       <c r="D17" s="6">
-        <v>102.704017348527</v>
+        <v>101.119529294733</v>
       </c>
       <c r="E17" s="6">
-        <v>3192.6836997723999</v>
+        <v>3201.7396906396598</v>
       </c>
       <c r="F17" s="6">
-        <v>3411.9149606606502</v>
+        <v>3417.0420945701198</v>
       </c>
       <c r="G17" s="6">
-        <v>3596.1696352049298</v>
+        <v>3599.6593534027702</v>
       </c>
       <c r="H17" s="6">
-        <v>1.00162827139077</v>
-      </c>
-      <c r="I17" s="6">
-        <v>28000</v>
+        <v>1.0014539587050999</v>
+      </c>
+      <c r="I17" s="18">
+        <v>4300</v>
       </c>
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
@@ -1577,30 +1591,30 @@
       <c r="N17" s="13"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="19"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="6">
-        <v>0.28868655948048799</v>
+        <v>0.28730248791936702</v>
       </c>
       <c r="D18" s="6">
-        <v>3.8497412667615999E-2</v>
+        <v>3.1641590623498098E-2</v>
       </c>
       <c r="E18" s="6">
-        <v>0.21769316633765701</v>
+        <v>0.226749884476039</v>
       </c>
       <c r="F18" s="6">
-        <v>0.28910271138749599</v>
+        <v>0.28699387249675801</v>
       </c>
       <c r="G18" s="6">
-        <v>0.35816828159516101</v>
+        <v>0.35045813899238798</v>
       </c>
       <c r="H18" s="6">
-        <v>1.0013156008116999</v>
-      </c>
-      <c r="I18" s="6">
-        <v>63000</v>
+        <v>1.0020097379952799</v>
+      </c>
+      <c r="I18" s="18">
+        <v>2000</v>
       </c>
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
@@ -1609,30 +1623,30 @@
       <c r="N18" s="13"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="19"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="6">
-        <v>1.77429367345932E-2</v>
+        <v>1.6307940901295202E-2</v>
       </c>
       <c r="D19" s="6">
-        <v>2.39526344160777E-2</v>
+        <v>1.69220635345005E-2</v>
       </c>
       <c r="E19" s="6">
-        <v>5.2253464661805504E-3</v>
+        <v>5.17774668022003E-3</v>
       </c>
       <c r="F19" s="6">
-        <v>1.2053884502572399E-2</v>
+        <v>1.18598223691959E-2</v>
       </c>
       <c r="G19" s="6">
-        <v>6.6418169384802397E-2</v>
+        <v>5.4147273281863299E-2</v>
       </c>
       <c r="H19" s="6">
-        <v>1.00098860339158</v>
-      </c>
-      <c r="I19" s="6">
-        <v>84000</v>
+        <v>1.0009900219918599</v>
+      </c>
+      <c r="I19" s="18">
+        <v>110000</v>
       </c>
       <c r="J19" s="13"/>
       <c r="K19" s="13"/>
@@ -1641,30 +1655,30 @@
       <c r="N19" s="13"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="19"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="6">
-        <v>9920.7766520927598</v>
+        <v>10173.404875026599</v>
       </c>
       <c r="D20" s="6">
-        <v>9897.1747576228609</v>
+        <v>10098.4391822124</v>
       </c>
       <c r="E20" s="6">
-        <v>226.686781898758</v>
+        <v>341.07258825635</v>
       </c>
       <c r="F20" s="6">
-        <v>6882.4956933035501</v>
+        <v>7109.5748550213902</v>
       </c>
       <c r="G20" s="6">
-        <v>36624.3408184211</v>
+        <v>37300.821978334403</v>
       </c>
       <c r="H20" s="6">
-        <v>1.00098860339158</v>
-      </c>
-      <c r="I20" s="6">
-        <v>84000</v>
+        <v>1.0009900219918599</v>
+      </c>
+      <c r="I20" s="18">
+        <v>110000</v>
       </c>
       <c r="J20" s="13"/>
       <c r="K20" s="13"/>
@@ -1673,30 +1687,30 @@
       <c r="N20" s="13"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="19"/>
+      <c r="A21" s="23"/>
       <c r="B21" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="6">
-        <v>11.5175787683725</v>
+        <v>11.5677642207406</v>
       </c>
       <c r="D21" s="6">
-        <v>1.7133827404626101</v>
+        <v>1.74920482340329</v>
       </c>
       <c r="E21" s="6">
-        <v>8.6494399566885303</v>
+        <v>8.6561019017527503</v>
       </c>
       <c r="F21" s="6">
-        <v>11.3463017927638</v>
+        <v>11.3902152646162</v>
       </c>
       <c r="G21" s="6">
-        <v>15.3831515459953</v>
+        <v>15.526210796839599</v>
       </c>
       <c r="H21" s="6">
-        <v>1.00159769479973</v>
-      </c>
-      <c r="I21" s="6">
-        <v>5200</v>
+        <v>1.0013543857899201</v>
+      </c>
+      <c r="I21" s="18">
+        <v>5400</v>
       </c>
       <c r="J21" s="13"/>
       <c r="K21" s="13"/>
@@ -1705,30 +1719,30 @@
       <c r="N21" s="13"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="19"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C22" s="6">
-        <v>0.211383661199147</v>
+        <v>0.209737164163911</v>
       </c>
       <c r="D22" s="6">
-        <v>3.0632358028365898E-2</v>
+        <v>3.00061528396201E-2</v>
       </c>
       <c r="E22" s="6">
-        <v>0.16064344057225299</v>
+        <v>0.15983636810197799</v>
       </c>
       <c r="F22" s="6">
-        <v>0.20824511717602001</v>
+        <v>0.20671380713405399</v>
       </c>
       <c r="G22" s="6">
-        <v>0.28012953687405601</v>
+        <v>0.27726685859496603</v>
       </c>
       <c r="H22" s="6">
-        <v>1.00152509380659</v>
-      </c>
-      <c r="I22" s="6">
-        <v>21000</v>
+        <v>1.00139761253346</v>
+      </c>
+      <c r="I22" s="18">
+        <v>4900</v>
       </c>
       <c r="J22" s="13"/>
       <c r="K22" s="13"/>
@@ -1737,30 +1751,30 @@
       <c r="N22" s="13"/>
     </row>
     <row r="23" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
+      <c r="A23" s="24"/>
       <c r="B23" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C23" s="7">
-        <v>4.8271521366149397</v>
+        <v>4.8627020954009703</v>
       </c>
       <c r="D23" s="7">
-        <v>0.67934226519130003</v>
+        <v>0.67632000182020302</v>
       </c>
       <c r="E23" s="7">
-        <v>3.5697770794144801</v>
+        <v>3.6066337140595999</v>
       </c>
       <c r="F23" s="7">
-        <v>4.8020333612660098</v>
+        <v>4.8376062241043298</v>
       </c>
       <c r="G23" s="7">
-        <v>6.2249662758575397</v>
+        <v>6.2563984146710903</v>
       </c>
       <c r="H23" s="7">
-        <v>1.00152509380659</v>
-      </c>
-      <c r="I23" s="7">
-        <v>21000</v>
+        <v>1.00139761253346</v>
+      </c>
+      <c r="I23" s="19">
+        <v>4900</v>
       </c>
       <c r="J23" s="13"/>
       <c r="K23" s="13"/>
@@ -1769,32 +1783,32 @@
       <c r="N23" s="13"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="22" t="s">
         <v>11</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="6">
-        <v>74.441785551602905</v>
+        <v>73.686389627653796</v>
       </c>
       <c r="D24" s="6">
-        <v>31.007261462346701</v>
+        <v>4.9636433448424704</v>
       </c>
       <c r="E24" s="6">
-        <v>0.96101038366206204</v>
+        <v>61.782086328631998</v>
       </c>
       <c r="F24" s="6">
-        <v>74.915175397906197</v>
+        <v>73.780466354866505</v>
       </c>
       <c r="G24" s="6">
-        <v>141.11710555731901</v>
+        <v>83.303680280627006</v>
       </c>
       <c r="H24" s="6">
-        <v>1.0010104901147401</v>
-      </c>
-      <c r="I24" s="6">
-        <v>84000</v>
+        <v>1.0011045790497499</v>
+      </c>
+      <c r="I24" s="18">
+        <v>17000</v>
       </c>
       <c r="J24" s="13"/>
       <c r="K24" s="13"/>
@@ -1803,30 +1817,30 @@
       <c r="N24" s="13"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" s="19"/>
+      <c r="A25" s="23"/>
       <c r="B25" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C25" s="6">
-        <v>249.92128226507299</v>
+        <v>22.0244857550089</v>
       </c>
       <c r="D25" s="6">
-        <v>45369.718150050998</v>
+        <v>2002.45883858</v>
       </c>
       <c r="E25" s="6">
-        <v>1.2745507358633799E-2</v>
+        <v>1.1558582842024399E-2</v>
       </c>
       <c r="F25" s="6">
-        <v>1.33047639575006</v>
+        <v>0.50168259560384898</v>
       </c>
       <c r="G25" s="6">
-        <v>369.42527697750103</v>
+        <v>61.481172194248103</v>
       </c>
       <c r="H25" s="6">
-        <v>1.0009932116278899</v>
-      </c>
-      <c r="I25" s="6">
-        <v>84000</v>
+        <v>1.00102502844166</v>
+      </c>
+      <c r="I25" s="18">
+        <v>50000</v>
       </c>
       <c r="J25" s="13"/>
       <c r="K25" s="13"/>
@@ -1835,30 +1849,30 @@
       <c r="N25" s="13"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" s="19"/>
+      <c r="A26" s="23"/>
       <c r="B26" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C26" s="6">
-        <v>569.31518720949805</v>
+        <v>717.79236115381298</v>
       </c>
       <c r="D26" s="6">
-        <v>2373.1140814272499</v>
+        <v>2585.9912888222302</v>
       </c>
       <c r="E26" s="6">
-        <v>7.3273474377370399E-6</v>
+        <v>2.6455484636173597E-4</v>
       </c>
       <c r="F26" s="6">
-        <v>0.56491831089086697</v>
+        <v>3.9732137572889998</v>
       </c>
       <c r="G26" s="6">
-        <v>6155.8176130026404</v>
+        <v>7484.9830292245097</v>
       </c>
       <c r="H26" s="6">
-        <v>1.0009932116278899</v>
-      </c>
-      <c r="I26" s="6">
-        <v>84000</v>
+        <v>1.00102502844166</v>
+      </c>
+      <c r="I26" s="18">
+        <v>50000</v>
       </c>
       <c r="J26" s="13"/>
       <c r="K26" s="13"/>
@@ -1867,30 +1881,30 @@
       <c r="N26" s="13"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" s="19"/>
+      <c r="A27" s="23"/>
       <c r="B27" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C27" s="6">
-        <v>62.360959558118402</v>
+        <v>63.544495629650797</v>
       </c>
       <c r="D27" s="6">
-        <v>13.725077688255301</v>
+        <v>13.647393845094101</v>
       </c>
       <c r="E27" s="6">
-        <v>40.767362204679699</v>
+        <v>41.433574076686099</v>
       </c>
       <c r="F27" s="6">
-        <v>60.373845850278201</v>
+        <v>61.851406517314203</v>
       </c>
       <c r="G27" s="6">
-        <v>93.663889129401795</v>
+        <v>93.770814530840696</v>
       </c>
       <c r="H27" s="6">
-        <v>1.00238121418737</v>
-      </c>
-      <c r="I27" s="6">
-        <v>1400</v>
+        <v>1.00766172074369</v>
+      </c>
+      <c r="I27" s="18">
+        <v>300</v>
       </c>
       <c r="J27" s="13"/>
       <c r="K27" s="13"/>
@@ -1899,30 +1913,30 @@
       <c r="N27" s="13"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" s="19"/>
+      <c r="A28" s="23"/>
       <c r="B28" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C28" s="6">
-        <v>3849.87027953695</v>
+        <v>3848.00553722822</v>
       </c>
       <c r="D28" s="6">
-        <v>47.193651896700899</v>
+        <v>47.101367553986499</v>
       </c>
       <c r="E28" s="6">
-        <v>3759.0442636736302</v>
+        <v>3757.6239899315001</v>
       </c>
       <c r="F28" s="6">
-        <v>3849.3444856481501</v>
+        <v>3847.4985430239099</v>
       </c>
       <c r="G28" s="6">
-        <v>3944.70523908011</v>
+        <v>3941.9897234759501</v>
       </c>
       <c r="H28" s="6">
-        <v>1.0009979088367</v>
-      </c>
-      <c r="I28" s="6">
-        <v>41000</v>
+        <v>1.0012006997887</v>
+      </c>
+      <c r="I28" s="18">
+        <v>9300</v>
       </c>
       <c r="J28" s="13"/>
       <c r="K28" s="13"/>
@@ -1931,30 +1945,30 @@
       <c r="N28" s="13"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" s="19"/>
+      <c r="A29" s="23"/>
       <c r="B29" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C29" s="6">
-        <v>0.16658760156563601</v>
+        <v>0.173234801443788</v>
       </c>
       <c r="D29" s="6">
-        <v>1.55563493035486E-2</v>
+        <v>1.47722512131393E-2</v>
       </c>
       <c r="E29" s="6">
-        <v>0.13643300807813299</v>
+        <v>0.145158294731763</v>
       </c>
       <c r="F29" s="6">
-        <v>0.166406588201889</v>
+        <v>0.17287514102239401</v>
       </c>
       <c r="G29" s="6">
-        <v>0.19764443655250299</v>
+        <v>0.20316843494960499</v>
       </c>
       <c r="H29" s="6">
-        <v>1.0016652965756101</v>
-      </c>
-      <c r="I29" s="6">
-        <v>3200</v>
+        <v>1.0016802034415699</v>
+      </c>
+      <c r="I29" s="18">
+        <v>2900</v>
       </c>
       <c r="J29" s="13"/>
       <c r="K29" s="13"/>
@@ -1963,30 +1977,30 @@
       <c r="N29" s="13"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" s="19"/>
+      <c r="A30" s="23"/>
       <c r="B30" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C30" s="6">
-        <v>1.92122052831473E-2</v>
+        <v>2.0684621778474601E-2</v>
       </c>
       <c r="D30" s="6">
-        <v>3.0956588674514499E-3</v>
+        <v>3.05315100015215E-3</v>
       </c>
       <c r="E30" s="6">
-        <v>1.3444813970829E-2</v>
+        <v>1.5052580377224199E-2</v>
       </c>
       <c r="F30" s="6">
-        <v>1.9102178599923001E-2</v>
+        <v>2.0551585358500001E-2</v>
       </c>
       <c r="G30" s="6">
-        <v>2.5569172004589299E-2</v>
+        <v>2.6995474279545101E-2</v>
       </c>
       <c r="H30" s="6">
-        <v>1.00101543173385</v>
-      </c>
-      <c r="I30" s="6">
-        <v>8000</v>
+        <v>1.00286967413068</v>
+      </c>
+      <c r="I30" s="18">
+        <v>1100</v>
       </c>
       <c r="J30" s="13"/>
       <c r="K30" s="13"/>
@@ -1995,30 +2009,30 @@
       <c r="N30" s="13"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" s="19"/>
+      <c r="A31" s="23"/>
       <c r="B31" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C31" s="6">
-        <v>2940.6551582844399</v>
+        <v>2500.2768103011299</v>
       </c>
       <c r="D31" s="6">
-        <v>1053.96650200724</v>
+        <v>791.70922557805204</v>
       </c>
       <c r="E31" s="6">
-        <v>1529.56053858069</v>
+        <v>1372.2020889708101</v>
       </c>
       <c r="F31" s="6">
-        <v>2740.5277086117699</v>
+        <v>2367.6055080299402</v>
       </c>
       <c r="G31" s="6">
-        <v>5532.1048796755704</v>
+        <v>4413.44877383946</v>
       </c>
       <c r="H31" s="6">
-        <v>1.00101543173385</v>
-      </c>
-      <c r="I31" s="6">
-        <v>8000</v>
+        <v>1.00286967413068</v>
+      </c>
+      <c r="I31" s="18">
+        <v>1100</v>
       </c>
       <c r="J31" s="13"/>
       <c r="K31" s="13"/>
@@ -2027,30 +2041,30 @@
       <c r="N31" s="13"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" s="19"/>
+      <c r="A32" s="23"/>
       <c r="B32" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C32" s="6">
-        <v>17.707930693418799</v>
+        <v>18.401744608249299</v>
       </c>
       <c r="D32" s="6">
-        <v>3.9063708746669001</v>
+        <v>3.9494385216729202</v>
       </c>
       <c r="E32" s="6">
-        <v>11.610982113879</v>
+        <v>12.038326961575301</v>
       </c>
       <c r="F32" s="6">
-        <v>17.120576207210199</v>
+        <v>17.894420935929201</v>
       </c>
       <c r="G32" s="6">
-        <v>26.6399705329443</v>
+        <v>27.117770782073102</v>
       </c>
       <c r="H32" s="6">
-        <v>1.0020295309465601</v>
-      </c>
-      <c r="I32" s="6">
-        <v>1600</v>
+        <v>1.00790521339495</v>
+      </c>
+      <c r="I32" s="18">
+        <v>290</v>
       </c>
       <c r="J32" s="13"/>
       <c r="K32" s="13"/>
@@ -2059,30 +2073,30 @@
       <c r="N32" s="13"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A33" s="19"/>
+      <c r="A33" s="23"/>
       <c r="B33" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C33" s="6">
-        <v>0.118493685748324</v>
+        <v>0.118758948064538</v>
       </c>
       <c r="D33" s="6">
-        <v>9.4052443421735795E-3</v>
+        <v>9.4449515851099397E-3</v>
       </c>
       <c r="E33" s="6">
-        <v>0.10087446587409001</v>
+        <v>0.101108032070756</v>
       </c>
       <c r="F33" s="6">
-        <v>0.118202401105327</v>
+        <v>0.11844159858094</v>
       </c>
       <c r="G33" s="6">
-        <v>0.13768589720337099</v>
+        <v>0.138075755086632</v>
       </c>
       <c r="H33" s="6">
-        <v>1.0009902251317899</v>
-      </c>
-      <c r="I33" s="6">
-        <v>84000</v>
+        <v>1.0010885534129299</v>
+      </c>
+      <c r="I33" s="18">
+        <v>19000</v>
       </c>
       <c r="J33" s="13"/>
       <c r="K33" s="13"/>
@@ -2091,30 +2105,30 @@
       <c r="N33" s="13"/>
     </row>
     <row r="34" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="20"/>
+      <c r="A34" s="24"/>
       <c r="B34" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C34" s="7">
-        <v>8.4926609416191408</v>
+        <v>8.4738479051686308</v>
       </c>
       <c r="D34" s="7">
-        <v>0.67694385824257797</v>
+        <v>0.67598076249136696</v>
       </c>
       <c r="E34" s="7">
-        <v>7.2629079688744902</v>
+        <v>7.24240109621402</v>
       </c>
       <c r="F34" s="7">
-        <v>8.4600650295498099</v>
+        <v>8.4429795948475093</v>
       </c>
       <c r="G34" s="7">
-        <v>9.9133114741661998</v>
+        <v>9.8904110733773596</v>
       </c>
       <c r="H34" s="7">
-        <v>1.0009902251317899</v>
-      </c>
-      <c r="I34" s="7">
-        <v>84000</v>
+        <v>1.0010885534129299</v>
+      </c>
+      <c r="I34" s="19">
+        <v>19000</v>
       </c>
       <c r="J34" s="13"/>
       <c r="K34" s="13"/>
@@ -2123,31 +2137,31 @@
       <c r="N34" s="13"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A35" s="18" t="s">
+      <c r="A35" s="22" t="s">
         <v>13</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C35" s="9">
-        <v>74.237715895352693</v>
+        <v>73.674950090339905</v>
       </c>
       <c r="D35" s="9">
-        <v>30.902627542136699</v>
+        <v>5.0831065884845597</v>
       </c>
       <c r="E35" s="9">
-        <v>0.49318095704850701</v>
+        <v>61.868241637780699</v>
       </c>
       <c r="F35" s="9">
-        <v>74.676824353257103</v>
+        <v>73.713516914245702</v>
       </c>
       <c r="G35" s="9">
-        <v>140.69192969502001</v>
+        <v>83.532798815076305</v>
       </c>
       <c r="H35" s="9">
-        <v>1.0009974816476099</v>
-      </c>
-      <c r="I35" s="9">
+        <v>1.0010646860843</v>
+      </c>
+      <c r="I35" s="20">
         <v>25000</v>
       </c>
       <c r="J35" s="13"/>
@@ -2157,30 +2171,30 @@
       <c r="N35" s="13"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A36" s="19"/>
+      <c r="A36" s="23"/>
       <c r="B36" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C36" s="11">
-        <v>77.139495624279803</v>
+        <v>15.5664339080822</v>
       </c>
       <c r="D36" s="11">
-        <v>2436.2790438150701</v>
+        <v>512.35668407482399</v>
       </c>
       <c r="E36" s="11">
-        <v>1.2577142852755E-2</v>
+        <v>1.1648646400341699E-2</v>
       </c>
       <c r="F36" s="11">
-        <v>1.3009491819289101</v>
+        <v>0.50203439771900804</v>
       </c>
       <c r="G36" s="11">
-        <v>351.699392897157</v>
+        <v>59.341882149399098</v>
       </c>
       <c r="H36" s="11">
-        <v>1.0009880565259699</v>
-      </c>
-      <c r="I36" s="11">
-        <v>84000</v>
+        <v>1.0010159256487301</v>
+      </c>
+      <c r="I36" s="21">
+        <v>65000</v>
       </c>
       <c r="J36" s="13"/>
       <c r="K36" s="13"/>
@@ -2189,30 +2203,30 @@
       <c r="N36" s="13"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A37" s="19"/>
+      <c r="A37" s="23"/>
       <c r="B37" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C37" s="11">
-        <v>576.31542038086002</v>
+        <v>714.71054255490401</v>
       </c>
       <c r="D37" s="11">
-        <v>2356.4278017070401</v>
+        <v>2567.9061383303601</v>
       </c>
       <c r="E37" s="11">
-        <v>8.0845669658076806E-6</v>
+        <v>2.8397320727629099E-4</v>
       </c>
       <c r="F37" s="11">
-        <v>0.59085285080878702</v>
+        <v>3.96764722535764</v>
       </c>
       <c r="G37" s="11">
-        <v>6321.7310089252196</v>
+        <v>7369.68754723454</v>
       </c>
       <c r="H37" s="11">
-        <v>1.0009880565259699</v>
-      </c>
-      <c r="I37" s="11">
-        <v>84000</v>
+        <v>1.0010159256487301</v>
+      </c>
+      <c r="I37" s="21">
+        <v>65000</v>
       </c>
       <c r="J37" s="13"/>
       <c r="K37" s="13"/>
@@ -2221,30 +2235,30 @@
       <c r="N37" s="13"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A38" s="19"/>
+      <c r="A38" s="23"/>
       <c r="B38" s="10" t="s">
         <v>15</v>
       </c>
       <c r="C38" s="11">
-        <v>33.427472474058597</v>
+        <v>32.943886103840001</v>
       </c>
       <c r="D38" s="11">
-        <v>3.7843298618957601</v>
+        <v>3.6800205129224399</v>
       </c>
       <c r="E38" s="11">
-        <v>26.653411881664098</v>
+        <v>26.4053119460727</v>
       </c>
       <c r="F38" s="11">
-        <v>33.188048679731203</v>
+        <v>32.715908747845901</v>
       </c>
       <c r="G38" s="11">
-        <v>41.498211431418</v>
+        <v>40.803880589167697</v>
       </c>
       <c r="H38" s="11">
-        <v>1.0010283710040599</v>
-      </c>
-      <c r="I38" s="11">
-        <v>13000</v>
+        <v>1.0011032333874601</v>
+      </c>
+      <c r="I38" s="21">
+        <v>17000</v>
       </c>
       <c r="J38" s="13"/>
       <c r="K38" s="13"/>
@@ -2253,30 +2267,30 @@
       <c r="N38" s="13"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A39" s="19"/>
+      <c r="A39" s="23"/>
       <c r="B39" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C39" s="11">
-        <v>3988.0840173205902</v>
+        <v>3988.9216892988402</v>
       </c>
       <c r="D39" s="11">
-        <v>39.9515795253836</v>
+        <v>40.169578743134501</v>
       </c>
       <c r="E39" s="11">
-        <v>3912.4819872451499</v>
+        <v>3913.7719888526999</v>
       </c>
       <c r="F39" s="11">
-        <v>3987.1565649498798</v>
+        <v>3987.8356503923501</v>
       </c>
       <c r="G39" s="11">
-        <v>4068.8104894932999</v>
+        <v>4070.7026095513102</v>
       </c>
       <c r="H39" s="11">
-        <v>1.0009949604055</v>
-      </c>
-      <c r="I39" s="11">
-        <v>34000</v>
+        <v>1.00102023945624</v>
+      </c>
+      <c r="I39" s="21">
+        <v>57000</v>
       </c>
       <c r="J39" s="13"/>
       <c r="K39" s="13"/>
@@ -2285,30 +2299,30 @@
       <c r="N39" s="13"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A40" s="19"/>
+      <c r="A40" s="23"/>
       <c r="B40" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C40" s="11">
-        <v>0.16360064716564099</v>
+        <v>0.175346807402154</v>
       </c>
       <c r="D40" s="11">
-        <v>2.9734048544961401E-2</v>
+        <v>2.62107353127655E-2</v>
       </c>
       <c r="E40" s="11">
-        <v>0.102633920240911</v>
+        <v>0.13001213708912199</v>
       </c>
       <c r="F40" s="11">
-        <v>0.164300939605249</v>
+        <v>0.173833201765317</v>
       </c>
       <c r="G40" s="11">
-        <v>0.215598604038053</v>
+        <v>0.230514025890278</v>
       </c>
       <c r="H40" s="11">
-        <v>1.0010122938534101</v>
-      </c>
-      <c r="I40" s="11">
-        <v>84000</v>
+        <v>1.00102491983653</v>
+      </c>
+      <c r="I40" s="21">
+        <v>50000</v>
       </c>
       <c r="J40" s="13"/>
       <c r="K40" s="13"/>
@@ -2317,30 +2331,30 @@
       <c r="N40" s="13"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A41" s="19"/>
+      <c r="A41" s="23"/>
       <c r="B41" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C41" s="11">
-        <v>1.7629710076494502E-2</v>
+        <v>1.68804288854561E-2</v>
       </c>
       <c r="D41" s="11">
-        <v>2.1828932226359701E-2</v>
+        <v>1.8959625298408202E-2</v>
       </c>
       <c r="E41" s="11">
-        <v>5.2198130265707398E-3</v>
+        <v>5.1962291132643104E-3</v>
       </c>
       <c r="F41" s="11">
-        <v>1.2115126011400299E-2</v>
+        <v>1.1984523281965601E-2</v>
       </c>
       <c r="G41" s="11">
-        <v>6.5020233056019103E-2</v>
+        <v>5.9072592046406899E-2</v>
       </c>
       <c r="H41" s="11">
-        <v>1.0010052831810601</v>
-      </c>
-      <c r="I41" s="11">
-        <v>84000</v>
+        <v>1.00099947875755</v>
+      </c>
+      <c r="I41" s="21">
+        <v>110000</v>
       </c>
       <c r="J41" s="13"/>
       <c r="K41" s="13"/>
@@ -2349,30 +2363,30 @@
       <c r="N41" s="13"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A42" s="19"/>
+      <c r="A42" s="23"/>
       <c r="B42" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C42" s="11">
-        <v>9901.1923719504503</v>
+        <v>10041.0393306319</v>
       </c>
       <c r="D42" s="11">
-        <v>9929.8825201017007</v>
+        <v>10026.1428191295</v>
       </c>
       <c r="E42" s="11">
-        <v>236.53910887364799</v>
+        <v>286.568166240577</v>
       </c>
       <c r="F42" s="11">
-        <v>6813.0900426981498</v>
+        <v>6962.39202627942</v>
       </c>
       <c r="G42" s="11">
-        <v>36702.031722168402</v>
+        <v>37035.943794224702</v>
       </c>
       <c r="H42" s="11">
-        <v>1.0010052831810601</v>
-      </c>
-      <c r="I42" s="11">
-        <v>84000</v>
+        <v>1.00099947875755</v>
+      </c>
+      <c r="I42" s="21">
+        <v>110000</v>
       </c>
       <c r="J42" s="13"/>
       <c r="K42" s="13"/>
@@ -2381,30 +2395,30 @@
       <c r="N42" s="13"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A43" s="19"/>
+      <c r="A43" s="23"/>
       <c r="B43" s="10" t="s">
         <v>17</v>
       </c>
       <c r="C43" s="11">
-        <v>9.3837226207353694</v>
+        <v>9.4021471343513703</v>
       </c>
       <c r="D43" s="11">
-        <v>0.99192571453407796</v>
+        <v>0.99992462555823103</v>
       </c>
       <c r="E43" s="11">
-        <v>7.6015601952688296</v>
+        <v>7.6137636916471596</v>
       </c>
       <c r="F43" s="11">
-        <v>9.3237308887312</v>
+        <v>9.3459313261440595</v>
       </c>
       <c r="G43" s="11">
-        <v>11.4965132422171</v>
+        <v>11.5258870293593</v>
       </c>
       <c r="H43" s="11">
-        <v>1.0009861321115601</v>
-      </c>
-      <c r="I43" s="11">
-        <v>21000</v>
+        <v>1.00103698523454</v>
+      </c>
+      <c r="I43" s="21">
+        <v>38000</v>
       </c>
       <c r="J43" s="13"/>
       <c r="K43" s="13"/>
@@ -2413,30 +2427,30 @@
       <c r="N43" s="13"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A44" s="19"/>
+      <c r="A44" s="23"/>
       <c r="B44" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C44" s="11">
-        <v>9.9058022407764096E-2</v>
+        <v>9.8965249430034694E-2</v>
       </c>
       <c r="D44" s="11">
-        <v>7.1684529615559101E-3</v>
+        <v>7.1970706339754597E-3</v>
       </c>
       <c r="E44" s="11">
-        <v>8.5579363090518598E-2</v>
+        <v>8.5323183844931594E-2</v>
       </c>
       <c r="F44" s="11">
-        <v>9.8869094517842093E-2</v>
+        <v>9.8794454358387601E-2</v>
       </c>
       <c r="G44" s="11">
-        <v>0.113578318242195</v>
+        <v>0.11353649048066899</v>
       </c>
       <c r="H44" s="11">
-        <v>1.0009934074839</v>
-      </c>
-      <c r="I44" s="11">
-        <v>45000</v>
+        <v>1.00099214176618</v>
+      </c>
+      <c r="I44" s="21">
+        <v>110000</v>
       </c>
       <c r="J44" s="13"/>
       <c r="K44" s="13"/>
@@ -2445,30 +2459,30 @@
       <c r="N44" s="13"/>
     </row>
     <row r="45" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="20"/>
+      <c r="A45" s="24"/>
       <c r="B45" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C45" s="7">
-        <v>10.148176813325501</v>
+        <v>10.1583474300096</v>
       </c>
       <c r="D45" s="7">
-        <v>0.73738427302545595</v>
+        <v>0.74364385773430997</v>
       </c>
       <c r="E45" s="7">
-        <v>8.8044973325594693</v>
+        <v>8.8077409805992399</v>
       </c>
       <c r="F45" s="7">
-        <v>10.114384124551099</v>
+        <v>10.122025638933</v>
       </c>
       <c r="G45" s="7">
-        <v>11.685060087936</v>
+        <v>11.720143985923301</v>
       </c>
       <c r="H45" s="7">
-        <v>1.0009934074839</v>
-      </c>
-      <c r="I45" s="7">
-        <v>45000</v>
+        <v>1.00099214176618</v>
+      </c>
+      <c r="I45" s="19">
+        <v>110000</v>
       </c>
       <c r="J45" s="13"/>
       <c r="K45" s="13"/>

</xml_diff>